<commit_message>
Sprint review 2 und 3, Project Diary Update
</commit_message>
<xml_diff>
--- a/Org/Sprint_Review_Protocol2.xlsx
+++ b/Org/Sprint_Review_Protocol2.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Felix Hadinger</t>
   </si>
   <si>
-    <t>Katarina Gmeiner</t>
-  </si>
-  <si>
     <t>Karim Salem</t>
   </si>
   <si>
@@ -121,7 +118,25 @@
     <t>Lilly Treml</t>
   </si>
   <si>
-    <t>Unity mit VR Brille verknüpfen</t>
+    <t>Organisation VR Brillen</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Recherge rund um VR in Unity</t>
+  </si>
+  <si>
+    <t>Test Libraries mit VR Support</t>
+  </si>
+  <si>
+    <t>VR Umgebung aufsetzen + mit DICOM Library verknüpfen</t>
+  </si>
+  <si>
+    <t>durch eine Intensive Prüfungsphasen konnten wir nicht so viel Zeit wie geplant investieren, werden das Item in nächsten Sprint übernehmen</t>
   </si>
 </sst>
 </file>
@@ -358,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -373,11 +388,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -385,6 +421,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -394,47 +457,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +777,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -769,28 +793,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -804,133 +828,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22">
+      <c r="B4" s="18"/>
+      <c r="C4" s="21">
         <v>2</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="24">
+      <c r="B5" s="20"/>
+      <c r="C5" s="23">
         <v>41948</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="25">
+      <c r="B6" s="20"/>
+      <c r="C6" s="24">
         <v>16</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -963,30 +987,46 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C16" s="7">
+        <v>60</v>
+      </c>
+      <c r="D16" s="7">
+        <v>10</v>
+      </c>
       <c r="E16" s="9">
         <f>D16-C16</f>
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
       <c r="E17" s="9">
         <f t="shared" ref="E17:E25" si="0">D17-C17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
     </row>
@@ -994,14 +1034,22 @@
       <c r="A18" s="8">
         <v>3</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7">
+        <v>7</v>
+      </c>
+      <c r="D18" s="7">
+        <v>5</v>
+      </c>
       <c r="E18" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>-2</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
@@ -1009,14 +1057,22 @@
       <c r="A19" s="8">
         <v>4</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6</v>
+      </c>
       <c r="E19" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
@@ -1120,7 +1176,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
-        <v>0</v>
+        <v>-51</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -1145,6 +1201,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1159,12 +1221,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>